<commit_message>
add download suppliers orders
</commit_message>
<xml_diff>
--- a/static/inventory.xlsx
+++ b/static/inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,10 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Location</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
           <t>Measurement</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Quantity</t>
         </is>
@@ -458,41 +453,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Соль</t>
+          <t>Курица</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Стеллаж 2</t>
+          <t>л</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>шт</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Тунец</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Холодильник 2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>кг</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>3</v>
+      <c r="C2" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>